<commit_message>
Updated Excel with Test Data
</commit_message>
<xml_diff>
--- a/Automation/Excel/configs/Test_Runner.xlsx
+++ b/Automation/Excel/configs/Test_Runner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitRepos\python-learning\Automation\Excel\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDD8864-D963-43A2-9AF9-585682618A86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93A04C4-FA38-459D-AEC9-B17B37C7449E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>EXECUTION STATE (Y/N)</t>
   </si>
@@ -73,13 +73,43 @@
   </si>
   <si>
     <t>test_case_10</t>
+  </si>
+  <si>
+    <t>TEST1@USER1.pfx</t>
+  </si>
+  <si>
+    <t>TEST2@USER2.pfx</t>
+  </si>
+  <si>
+    <t>TEST3@USER3.pfx</t>
+  </si>
+  <si>
+    <t>TEST4@USER4.pfx</t>
+  </si>
+  <si>
+    <t>TEST5@USER5.pfx</t>
+  </si>
+  <si>
+    <t>TEST6@USER6.pfx</t>
+  </si>
+  <si>
+    <t>TEST7@USER7.pfx</t>
+  </si>
+  <si>
+    <t>TEST8@USER8.pfx</t>
+  </si>
+  <si>
+    <t>TEST9@USER9.pfx</t>
+  </si>
+  <si>
+    <t>TEST10@USER10.pfx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +127,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,10 +178,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -155,8 +194,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -438,7 +479,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,7 +488,7 @@
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
@@ -480,7 +521,9 @@
       <c r="D2" s="4">
         <v>2</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="5" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -495,7 +538,9 @@
       <c r="D3" s="4">
         <v>4</v>
       </c>
-      <c r="E3" s="1"/>
+      <c r="E3" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
@@ -510,7 +555,9 @@
       <c r="D4" s="4">
         <v>2</v>
       </c>
-      <c r="E4" s="1"/>
+      <c r="E4" s="5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
@@ -525,7 +572,9 @@
       <c r="D5" s="4">
         <v>3</v>
       </c>
-      <c r="E5" s="1"/>
+      <c r="E5" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
@@ -540,7 +589,9 @@
       <c r="D6" s="4">
         <v>5</v>
       </c>
-      <c r="E6" s="1"/>
+      <c r="E6" s="5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
@@ -555,7 +606,9 @@
       <c r="D7" s="4">
         <v>2</v>
       </c>
-      <c r="E7" s="1"/>
+      <c r="E7" s="5" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
@@ -570,7 +623,9 @@
       <c r="D8" s="4">
         <v>1</v>
       </c>
-      <c r="E8" s="1"/>
+      <c r="E8" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
@@ -585,7 +640,9 @@
       <c r="D9" s="4">
         <v>5</v>
       </c>
-      <c r="E9" s="1"/>
+      <c r="E9" s="5" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
@@ -600,7 +657,9 @@
       <c r="D10" s="4">
         <v>6</v>
       </c>
-      <c r="E10" s="1"/>
+      <c r="E10" s="5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -615,10 +674,24 @@
       <c r="D11" s="4">
         <v>1</v>
       </c>
-      <c r="E11" s="1"/>
+      <c r="E11" s="5" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{C845D5DB-5E7E-429D-AC18-EC25E6E554E4}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{38C4E559-F788-4943-81CB-35040F084A15}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{5BE5AF47-1BBD-4CD9-894F-4B19A0E43096}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{F4D14FB6-2546-49EE-8F81-B1FFB26806C1}"/>
+    <hyperlink ref="E8" r:id="rId5" xr:uid="{482BDA07-13D1-4F34-B265-C432738254F1}"/>
+    <hyperlink ref="E10" r:id="rId6" xr:uid="{3670209D-5B00-4BB7-A624-C86FA1866B20}"/>
+    <hyperlink ref="E5" r:id="rId7" xr:uid="{2E49F3AF-2558-4560-B6C5-E1FF8E00490E}"/>
+    <hyperlink ref="E7" r:id="rId8" xr:uid="{7B400396-91C9-43F9-8BDD-45FD41EC6E24}"/>
+    <hyperlink ref="E9" r:id="rId9" xr:uid="{A5598CB0-9ACC-418C-B67B-8C04FFA47F71}"/>
+    <hyperlink ref="E11" r:id="rId10" xr:uid="{8C29740A-B3ED-48E0-9788-97E680995728}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finally the expected logic implemented, but this holds good for cases with status Y. I need to update the code for N status which should be marked as skipped in HTML Report.
</commit_message>
<xml_diff>
--- a/Automation/Excel/configs/Test_Runner.xlsx
+++ b/Automation/Excel/configs/Test_Runner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitRepos\python-learning\Automation\Excel\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B93A04C4-FA38-459D-AEC9-B17B37C7449E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C196C2A2-8665-44FB-9607-1C58E04A42D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>EXECUTION STATE (Y/N)</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>TEST10@USER10.pfx</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -479,7 +482,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,7 +547,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="B4" s="4">
         <v>3</v>
@@ -553,7 +556,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>18</v>
@@ -693,5 +696,6 @@
     <hyperlink ref="E11" r:id="rId10" xr:uid="{8C29740A-B3ED-48E0-9788-97E680995728}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Code Complete: User can run bulk cases and html report can generate one single consolidated file
</commit_message>
<xml_diff>
--- a/Automation/Excel/configs/Test_Runner.xlsx
+++ b/Automation/Excel/configs/Test_Runner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitRepos\python-learning\Automation\Excel\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C196C2A2-8665-44FB-9607-1C58E04A42D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91F801F-A85C-44E1-95A0-60FBCF8CF9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>EXECUTION STATE (Y/N)</t>
   </si>
@@ -40,9 +40,6 @@
   </si>
   <si>
     <t>CERTIFICATE</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>test_case_01</t>
@@ -482,7 +479,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,172 +510,172 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" s="4">
         <v>2</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B3" s="4">
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="4">
         <v>4</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="4">
         <v>3</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="4">
         <v>3</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="4">
         <v>3</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B6" s="4">
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" s="4">
         <v>5</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B7" s="4">
         <v>6</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="4">
         <v>2</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B8" s="4">
         <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" s="4">
         <v>1</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B9" s="4">
         <v>8</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" s="4">
         <v>5</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B10" s="4">
         <v>9</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" s="4">
         <v>6</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="B11" s="4">
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
code will now scan sub-directories as well
</commit_message>
<xml_diff>
--- a/Automation/Excel/configs/Test_Runner.xlsx
+++ b/Automation/Excel/configs/Test_Runner.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitRepos\python-learning\Automation\Excel\configs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E91F801F-A85C-44E1-95A0-60FBCF8CF9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97458515-820B-43D6-ABDE-65484540FA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>EXECUTION STATE (Y/N)</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -479,7 +482,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -595,7 +598,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4">
         <v>6</v>
@@ -612,7 +615,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" s="4">
         <v>7</v>
@@ -629,7 +632,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="4">
         <v>8</v>
@@ -646,7 +649,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="4">
         <v>9</v>
@@ -663,7 +666,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4">
         <v>10</v>

</xml_diff>